<commit_message>
Auto stash before checking out "HEAD"
</commit_message>
<xml_diff>
--- a/2. WBS/5조_WBS_현대이지웰_최종프로젝트.xlsx
+++ b/2. WBS/5조_WBS_현대이지웰_최종프로젝트.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redgu\OneDrive\Desktop\related_Re_View\Re_View_Doc\2. WBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC8A8D1-A363-4BA5-AD96-68C412FF5609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83CF6DD-8ABB-4C8B-ADA1-D4D6475F7FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="285" yWindow="555" windowWidth="21315" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="159">
   <si>
     <t>팀명</t>
   </si>
@@ -1334,6 +1334,32 @@
     <t>전체 페이지</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">바우만 타입 게시판 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>UI</t>
+    </r>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>바우만 타입 게시판 시스템</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1342,7 +1368,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="45">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1633,6 +1659,20 @@
       <color theme="7"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
       <charset val="129"/>
     </font>
   </fonts>
@@ -2249,7 +2289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2674,7 +2714,34 @@
     <xf numFmtId="0" fontId="23" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="21" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="8" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2901,10 +2968,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BO90"/>
+  <dimension ref="A1:BO92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58:G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -7154,11 +7221,11 @@
         <v>128</v>
       </c>
       <c r="C50" s="44" t="str">
-        <f t="shared" ref="C50:C69" ca="1" si="12">IF(F50=E50, IF(TODAY()&gt;F50, "100%", "0%"), ROUND(MAX(0, MIN(TODAY(), F50) - E50) / (F50 - E50) * 100, 1) &amp; "%")</f>
+        <f t="shared" ref="C50:C71" ca="1" si="12">IF(F50=E50, IF(TODAY()&gt;F50, "100%", "0%"), ROUND(MAX(0, MIN(TODAY(), F50) - E50) / (F50 - E50) * 100, 1) &amp; "%")</f>
         <v>100%</v>
       </c>
       <c r="D50" s="104" t="str">
-        <f t="shared" ref="D50:D69" si="13">IF(AND(F50&lt;&gt;"", E50&lt;&gt;""), F50 - E50 + 1 &amp; "일", "")</f>
+        <f t="shared" ref="D50:D71" si="13">IF(AND(F50&lt;&gt;"", E50&lt;&gt;""), F50 - E50 + 1 &amp; "일", "")</f>
         <v>7일</v>
       </c>
       <c r="E50" s="45">
@@ -7399,14 +7466,14 @@
     </row>
     <row r="53" spans="1:67" ht="15.75" customHeight="1" thickBot="1">
       <c r="A53" s="124"/>
-      <c r="B53" s="141" t="s">
+      <c r="B53" s="144" t="s">
         <v>156</v>
       </c>
       <c r="C53" s="141"/>
       <c r="D53" s="141"/>
       <c r="E53" s="141"/>
       <c r="F53" s="141"/>
-      <c r="G53" s="141"/>
+      <c r="G53" s="145"/>
       <c r="H53" s="103"/>
       <c r="I53" s="60"/>
       <c r="J53" s="60"/>
@@ -7470,24 +7537,24 @@
     </row>
     <row r="54" spans="1:67" ht="15" customHeight="1" thickBot="1">
       <c r="A54" s="124"/>
-      <c r="B54" s="87" t="s">
+      <c r="B54" s="100" t="s">
         <v>150</v>
       </c>
       <c r="C54" s="47" t="str">
         <f t="shared" ref="C54" ca="1" si="16">IF(F54=E54, IF(TODAY()&gt;F54, "100%", "0%"), ROUND(MAX(0, MIN(TODAY(), F54) - E54) / (F54 - E54) * 100, 1) &amp; "%")</f>
         <v>100%</v>
       </c>
-      <c r="D54" s="40" t="str">
+      <c r="D54" s="142" t="str">
         <f t="shared" ref="D54" si="17">IF(AND(F54&lt;&gt;"", E54&lt;&gt;""), F54 - E54 + 1 &amp; "일", "")</f>
         <v>2일</v>
       </c>
-      <c r="E54" s="41">
+      <c r="E54" s="48">
         <v>45980</v>
       </c>
-      <c r="F54" s="41">
+      <c r="F54" s="48">
         <v>45981</v>
       </c>
-      <c r="G54" s="142" t="s">
+      <c r="G54" s="143" t="s">
         <v>117</v>
       </c>
       <c r="H54" s="59"/>
@@ -7724,14 +7791,18 @@
       </c>
       <c r="C57" s="20" t="str">
         <f ca="1">IF(F57=E57, IF(TODAY()&gt;F57, "100%", "0%"), ROUND(MAX(0, MIN(TODAY(), F57) - E57) / (F57 - E57) * 100, 1) &amp; "%")</f>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="D57" s="21" t="str">
         <f>IF(AND(F57&lt;&gt;"", E57&lt;&gt;""), F57 - E57 + 1 &amp; "일", "")</f>
-        <v/>
-      </c>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
+        <v>14일</v>
+      </c>
+      <c r="E57" s="22">
+        <v>45985</v>
+      </c>
+      <c r="F57" s="22">
+        <v>45998</v>
+      </c>
       <c r="G57" s="68" t="s">
         <v>134</v>
       </c>
@@ -7798,25 +7869,25 @@
     </row>
     <row r="58" spans="1:67" ht="15" customHeight="1" thickBot="1">
       <c r="A58" s="124"/>
-      <c r="B58" s="115" t="s">
-        <v>129</v>
-      </c>
-      <c r="C58" s="116" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>100%</v>
-      </c>
-      <c r="D58" s="117" t="str">
-        <f t="shared" si="13"/>
-        <v>3일</v>
-      </c>
-      <c r="E58" s="75">
-        <v>45980</v>
-      </c>
-      <c r="F58" s="75">
-        <v>45982</v>
-      </c>
-      <c r="G58" s="118" t="s">
-        <v>117</v>
+      <c r="B58" s="146" t="s">
+        <v>157</v>
+      </c>
+      <c r="C58" s="147" t="str">
+        <f ca="1">IF(F58=E58, IF(TODAY()&gt;F58, "100%", "0%"), ROUND(MAX(0, MIN(TODAY(), F58) - E58) / (F58 - E58) * 100, 1) &amp; "%")</f>
+        <v>0%</v>
+      </c>
+      <c r="D58" s="148" t="str">
+        <f>IF(AND(F58&lt;&gt;"", E58&lt;&gt;""), F58 - E58 + 1 &amp; "일", "")</f>
+        <v>10일</v>
+      </c>
+      <c r="E58" s="149">
+        <v>45989</v>
+      </c>
+      <c r="F58" s="149">
+        <v>45998</v>
+      </c>
+      <c r="G58" s="150" t="s">
+        <v>108</v>
       </c>
       <c r="H58" s="59"/>
       <c r="I58" s="60"/>
@@ -7881,20 +7952,26 @@
     </row>
     <row r="59" spans="1:67" ht="15" customHeight="1" thickBot="1">
       <c r="A59" s="124"/>
-      <c r="B59" s="94" t="s">
-        <v>130</v>
-      </c>
-      <c r="C59" s="32" t="str">
-        <f t="shared" ca="1" si="12"/>
+      <c r="B59" s="115" t="s">
+        <v>129</v>
+      </c>
+      <c r="C59" s="116" t="str">
+        <f ca="1">IF(F59=E59, IF(TODAY()&gt;F59, "100%", "0%"), ROUND(MAX(0, MIN(TODAY(), F59) - E59) / (F59 - E59) * 100, 1) &amp; "%")</f>
         <v>100%</v>
       </c>
-      <c r="D59" s="21" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="69"/>
+      <c r="D59" s="117" t="str">
+        <f>IF(AND(F59&lt;&gt;"", E59&lt;&gt;""), F59 - E59 + 1 &amp; "일", "")</f>
+        <v>3일</v>
+      </c>
+      <c r="E59" s="75">
+        <v>45980</v>
+      </c>
+      <c r="F59" s="75">
+        <v>45982</v>
+      </c>
+      <c r="G59" s="118" t="s">
+        <v>117</v>
+      </c>
       <c r="H59" s="59"/>
       <c r="I59" s="60"/>
       <c r="J59" s="60"/>
@@ -7956,22 +8033,28 @@
       <c r="BN59" s="60"/>
       <c r="BO59" s="60"/>
     </row>
-    <row r="60" spans="1:67" ht="15.75" customHeight="1" thickBot="1">
+    <row r="60" spans="1:67" ht="15" customHeight="1" thickBot="1">
       <c r="A60" s="124"/>
       <c r="B60" s="94" t="s">
-        <v>131</v>
-      </c>
-      <c r="C60" s="20" t="str">
+        <v>130</v>
+      </c>
+      <c r="C60" s="32" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="D60" s="21" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="69"/>
+        <f>IF(AND(F60&lt;&gt;"", E60&lt;&gt;""), F60 - E60 + 1 &amp; "일", "")</f>
+        <v>10일</v>
+      </c>
+      <c r="E60" s="22">
+        <v>45989</v>
+      </c>
+      <c r="F60" s="22">
+        <v>45998</v>
+      </c>
+      <c r="G60" s="69" t="s">
+        <v>119</v>
+      </c>
       <c r="H60" s="59"/>
       <c r="I60" s="60"/>
       <c r="J60" s="60"/>
@@ -8033,13 +8116,13 @@
       <c r="BN60" s="60"/>
       <c r="BO60" s="60"/>
     </row>
-    <row r="61" spans="1:67" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A61" s="125"/>
-      <c r="B61" s="95" t="s">
-        <v>149</v>
-      </c>
-      <c r="C61" s="20" t="str">
-        <f t="shared" ref="C61" ca="1" si="18">IF(F61=E61, IF(TODAY()&gt;F61, "100%", "0%"), ROUND(MAX(0, MIN(TODAY(), F61) - E61) / (F61 - E61) * 100, 1) &amp; "%")</f>
+    <row r="61" spans="1:67" ht="15" customHeight="1" thickBot="1">
+      <c r="A61" s="124"/>
+      <c r="B61" s="151" t="s">
+        <v>158</v>
+      </c>
+      <c r="C61" s="32" t="str">
+        <f t="shared" ca="1" si="12"/>
         <v>0%</v>
       </c>
       <c r="D61" s="21" t="str">
@@ -8052,8 +8135,8 @@
       <c r="F61" s="22">
         <v>45998</v>
       </c>
-      <c r="G61" s="68" t="s">
-        <v>117</v>
+      <c r="G61" s="69" t="s">
+        <v>107</v>
       </c>
       <c r="H61" s="59"/>
       <c r="I61" s="60"/>
@@ -8117,24 +8200,26 @@
       <c r="BO61" s="60"/>
     </row>
     <row r="62" spans="1:67" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A62" s="124" t="s">
-        <v>90</v>
-      </c>
-      <c r="B62" s="96" t="s">
-        <v>2</v>
+      <c r="A62" s="124"/>
+      <c r="B62" s="94" t="s">
+        <v>131</v>
       </c>
       <c r="C62" s="20" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="D62" s="21" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="E62" s="22"/>
-      <c r="F62" s="22"/>
-      <c r="G62" s="70" t="s">
-        <v>100</v>
+        <f>IF(AND(F62&lt;&gt;"", E62&lt;&gt;""), F62 - E62 + 1 &amp; "일", "")</f>
+        <v>10일</v>
+      </c>
+      <c r="E62" s="22">
+        <v>45989</v>
+      </c>
+      <c r="F62" s="22">
+        <v>45998</v>
+      </c>
+      <c r="G62" s="69" t="s">
+        <v>116</v>
       </c>
       <c r="H62" s="59"/>
       <c r="I62" s="60"/>
@@ -8197,23 +8282,27 @@
       <c r="BN62" s="60"/>
       <c r="BO62" s="60"/>
     </row>
-    <row r="63" spans="1:67" ht="15.75" thickBot="1">
-      <c r="A63" s="124"/>
-      <c r="B63" s="97" t="s">
-        <v>88</v>
-      </c>
-      <c r="C63" s="31" t="str">
-        <f t="shared" ref="C63" ca="1" si="19">IF(F63=E63, IF(TODAY()&gt;F63, "100%", "0%"), ROUND(MAX(0, MIN(TODAY(), F63) - E63) / (F63 - E63) * 100, 1) &amp; "%")</f>
-        <v>100%</v>
+    <row r="63" spans="1:67" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A63" s="125"/>
+      <c r="B63" s="95" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" s="20" t="str">
+        <f t="shared" ref="C63" ca="1" si="18">IF(F63=E63, IF(TODAY()&gt;F63, "100%", "0%"), ROUND(MAX(0, MIN(TODAY(), F63) - E63) / (F63 - E63) * 100, 1) &amp; "%")</f>
+        <v>0%</v>
       </c>
       <c r="D63" s="21" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="E63" s="22"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="70" t="s">
-        <v>100</v>
+        <f>IF(AND(F63&lt;&gt;"", E63&lt;&gt;""), F63 - E63 + 1 &amp; "일", "")</f>
+        <v>10일</v>
+      </c>
+      <c r="E63" s="22">
+        <v>45989</v>
+      </c>
+      <c r="F63" s="22">
+        <v>45998</v>
+      </c>
+      <c r="G63" s="68" t="s">
+        <v>117</v>
       </c>
       <c r="H63" s="59"/>
       <c r="I63" s="60"/>
@@ -8276,12 +8365,17 @@
       <c r="BN63" s="60"/>
       <c r="BO63" s="60"/>
     </row>
-    <row r="64" spans="1:67" ht="15.75" thickBot="1">
-      <c r="A64" s="124"/>
-      <c r="B64" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="C64" s="67"/>
+    <row r="64" spans="1:67" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A64" s="124" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" s="96" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="20" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v>100%</v>
+      </c>
       <c r="D64" s="21" t="str">
         <f t="shared" si="13"/>
         <v/>
@@ -8354,25 +8448,21 @@
     </row>
     <row r="65" spans="1:67" ht="15.75" thickBot="1">
       <c r="A65" s="124"/>
-      <c r="B65" s="81" t="s">
-        <v>90</v>
-      </c>
-      <c r="C65" s="35" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>0%</v>
-      </c>
-      <c r="D65" s="71" t="str">
+      <c r="B65" s="97" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" s="31" t="str">
+        <f t="shared" ref="C65" ca="1" si="19">IF(F65=E65, IF(TODAY()&gt;F65, "100%", "0%"), ROUND(MAX(0, MIN(TODAY(), F65) - E65) / (F65 - E65) * 100, 1) &amp; "%")</f>
+        <v>100%</v>
+      </c>
+      <c r="D65" s="21" t="str">
         <f t="shared" si="13"/>
-        <v>12일</v>
-      </c>
-      <c r="E65" s="36">
-        <v>45999</v>
-      </c>
-      <c r="F65" s="36">
-        <v>46010</v>
-      </c>
-      <c r="G65" s="37" t="s">
-        <v>98</v>
+        <v/>
+      </c>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="70" t="s">
+        <v>100</v>
       </c>
       <c r="H65" s="59"/>
       <c r="I65" s="60"/>
@@ -8435,27 +8525,20 @@
       <c r="BN65" s="60"/>
       <c r="BO65" s="60"/>
     </row>
-    <row r="66" spans="1:67" ht="15" customHeight="1" thickBot="1">
+    <row r="66" spans="1:67" ht="15.75" thickBot="1">
       <c r="A66" s="124"/>
-      <c r="B66" s="98" t="s">
-        <v>91</v>
-      </c>
-      <c r="C66" s="32" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>0%</v>
-      </c>
+      <c r="B66" s="97" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="67"/>
       <c r="D66" s="21" t="str">
         <f t="shared" si="13"/>
-        <v>10일</v>
-      </c>
-      <c r="E66" s="33">
-        <v>45999</v>
-      </c>
-      <c r="F66" s="33">
-        <v>46008</v>
-      </c>
-      <c r="G66" s="34" t="s">
-        <v>98</v>
+        <v/>
+      </c>
+      <c r="E66" s="22"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="70" t="s">
+        <v>100</v>
       </c>
       <c r="H66" s="59"/>
       <c r="I66" s="60"/>
@@ -8518,26 +8601,26 @@
       <c r="BN66" s="60"/>
       <c r="BO66" s="60"/>
     </row>
-    <row r="67" spans="1:67" ht="15.75" customHeight="1" thickBot="1">
+    <row r="67" spans="1:67" ht="15.75" thickBot="1">
       <c r="A67" s="124"/>
-      <c r="B67" s="95" t="s">
-        <v>3</v>
-      </c>
-      <c r="C67" s="20" t="str">
+      <c r="B67" s="81" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="35" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>0%</v>
       </c>
-      <c r="D67" s="21" t="str">
+      <c r="D67" s="71" t="str">
         <f t="shared" si="13"/>
-        <v>10일</v>
-      </c>
-      <c r="E67" s="22">
+        <v>12일</v>
+      </c>
+      <c r="E67" s="36">
         <v>45999</v>
       </c>
-      <c r="F67" s="22">
-        <v>46008</v>
-      </c>
-      <c r="G67" s="23" t="s">
+      <c r="F67" s="36">
+        <v>46010</v>
+      </c>
+      <c r="G67" s="37" t="s">
         <v>98</v>
       </c>
       <c r="H67" s="59"/>
@@ -8601,26 +8684,26 @@
       <c r="BN67" s="60"/>
       <c r="BO67" s="60"/>
     </row>
-    <row r="68" spans="1:67" ht="15.75" thickBot="1">
+    <row r="68" spans="1:67" ht="15" customHeight="1" thickBot="1">
       <c r="A68" s="124"/>
-      <c r="B68" s="95" t="s">
-        <v>92</v>
-      </c>
-      <c r="C68" s="20" t="str">
+      <c r="B68" s="98" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="32" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>0%</v>
       </c>
       <c r="D68" s="21" t="str">
         <f t="shared" si="13"/>
-        <v>1일</v>
-      </c>
-      <c r="E68" s="22">
-        <v>46010</v>
-      </c>
-      <c r="F68" s="22">
-        <v>46010</v>
-      </c>
-      <c r="G68" s="23" t="s">
+        <v>10일</v>
+      </c>
+      <c r="E68" s="33">
+        <v>45999</v>
+      </c>
+      <c r="F68" s="33">
+        <v>46008</v>
+      </c>
+      <c r="G68" s="34" t="s">
         <v>98</v>
       </c>
       <c r="H68" s="59"/>
@@ -8684,10 +8767,10 @@
       <c r="BN68" s="60"/>
       <c r="BO68" s="60"/>
     </row>
-    <row r="69" spans="1:67" ht="15.75" thickBot="1">
-      <c r="A69" s="125"/>
+    <row r="69" spans="1:67" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A69" s="124"/>
       <c r="B69" s="95" t="s">
-        <v>93</v>
+        <v>3</v>
       </c>
       <c r="C69" s="20" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -8695,13 +8778,13 @@
       </c>
       <c r="D69" s="21" t="str">
         <f t="shared" si="13"/>
-        <v>1일</v>
+        <v>10일</v>
       </c>
       <c r="E69" s="22">
-        <v>46010</v>
+        <v>45999</v>
       </c>
       <c r="F69" s="22">
-        <v>46010</v>
+        <v>46008</v>
       </c>
       <c r="G69" s="23" t="s">
         <v>98</v>
@@ -8767,15 +8850,175 @@
       <c r="BN69" s="60"/>
       <c r="BO69" s="60"/>
     </row>
-    <row r="70" spans="1:67">
-      <c r="E70" s="7"/>
-      <c r="F70" s="1"/>
-      <c r="I70" s="3"/>
+    <row r="70" spans="1:67" ht="15.75" thickBot="1">
+      <c r="A70" s="124"/>
+      <c r="B70" s="95" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" s="20" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v>0%</v>
+      </c>
+      <c r="D70" s="21" t="str">
+        <f t="shared" si="13"/>
+        <v>1일</v>
+      </c>
+      <c r="E70" s="22">
+        <v>46010</v>
+      </c>
+      <c r="F70" s="22">
+        <v>46010</v>
+      </c>
+      <c r="G70" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="H70" s="59"/>
+      <c r="I70" s="60"/>
+      <c r="J70" s="60"/>
+      <c r="K70" s="60"/>
+      <c r="L70" s="61"/>
+      <c r="M70" s="62"/>
+      <c r="N70" s="60"/>
+      <c r="O70" s="60"/>
+      <c r="P70" s="60"/>
+      <c r="Q70" s="60"/>
+      <c r="R70" s="60"/>
+      <c r="S70" s="61"/>
+      <c r="T70" s="62"/>
+      <c r="U70" s="60"/>
+      <c r="V70" s="60"/>
+      <c r="W70" s="60"/>
+      <c r="X70" s="60"/>
+      <c r="Y70" s="60"/>
+      <c r="Z70" s="61"/>
+      <c r="AA70" s="62"/>
+      <c r="AB70" s="60"/>
+      <c r="AC70" s="60"/>
+      <c r="AD70" s="60"/>
+      <c r="AE70" s="60"/>
+      <c r="AF70" s="60"/>
+      <c r="AG70" s="61"/>
+      <c r="AH70" s="62"/>
+      <c r="AI70" s="60"/>
+      <c r="AJ70" s="60"/>
+      <c r="AK70" s="60"/>
+      <c r="AL70" s="60"/>
+      <c r="AM70" s="60"/>
+      <c r="AN70" s="61"/>
+      <c r="AO70" s="62"/>
+      <c r="AP70" s="60"/>
+      <c r="AQ70" s="60"/>
+      <c r="AR70" s="60"/>
+      <c r="AS70" s="60"/>
+      <c r="AT70" s="60"/>
+      <c r="AU70" s="61"/>
+      <c r="AV70" s="62"/>
+      <c r="AW70" s="60"/>
+      <c r="AX70" s="60"/>
+      <c r="AY70" s="60"/>
+      <c r="AZ70" s="60"/>
+      <c r="BA70" s="60"/>
+      <c r="BB70" s="61"/>
+      <c r="BC70" s="62"/>
+      <c r="BD70" s="60"/>
+      <c r="BE70" s="60"/>
+      <c r="BF70" s="60"/>
+      <c r="BG70" s="60"/>
+      <c r="BH70" s="60"/>
+      <c r="BI70" s="61"/>
+      <c r="BJ70" s="62"/>
+      <c r="BK70" s="60"/>
+      <c r="BL70" s="60"/>
+      <c r="BM70" s="60"/>
+      <c r="BN70" s="60"/>
+      <c r="BO70" s="60"/>
     </row>
-    <row r="71" spans="1:67">
-      <c r="I71" s="3"/>
+    <row r="71" spans="1:67" ht="15.75" thickBot="1">
+      <c r="A71" s="125"/>
+      <c r="B71" s="95" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" s="20" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v>0%</v>
+      </c>
+      <c r="D71" s="21" t="str">
+        <f t="shared" si="13"/>
+        <v>1일</v>
+      </c>
+      <c r="E71" s="22">
+        <v>46010</v>
+      </c>
+      <c r="F71" s="22">
+        <v>46010</v>
+      </c>
+      <c r="G71" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="H71" s="59"/>
+      <c r="I71" s="60"/>
+      <c r="J71" s="60"/>
+      <c r="K71" s="60"/>
+      <c r="L71" s="61"/>
+      <c r="M71" s="62"/>
+      <c r="N71" s="60"/>
+      <c r="O71" s="60"/>
+      <c r="P71" s="60"/>
+      <c r="Q71" s="60"/>
+      <c r="R71" s="60"/>
+      <c r="S71" s="61"/>
+      <c r="T71" s="62"/>
+      <c r="U71" s="60"/>
+      <c r="V71" s="60"/>
+      <c r="W71" s="60"/>
+      <c r="X71" s="60"/>
+      <c r="Y71" s="60"/>
+      <c r="Z71" s="61"/>
+      <c r="AA71" s="62"/>
+      <c r="AB71" s="60"/>
+      <c r="AC71" s="60"/>
+      <c r="AD71" s="60"/>
+      <c r="AE71" s="60"/>
+      <c r="AF71" s="60"/>
+      <c r="AG71" s="61"/>
+      <c r="AH71" s="62"/>
+      <c r="AI71" s="60"/>
+      <c r="AJ71" s="60"/>
+      <c r="AK71" s="60"/>
+      <c r="AL71" s="60"/>
+      <c r="AM71" s="60"/>
+      <c r="AN71" s="61"/>
+      <c r="AO71" s="62"/>
+      <c r="AP71" s="60"/>
+      <c r="AQ71" s="60"/>
+      <c r="AR71" s="60"/>
+      <c r="AS71" s="60"/>
+      <c r="AT71" s="60"/>
+      <c r="AU71" s="61"/>
+      <c r="AV71" s="62"/>
+      <c r="AW71" s="60"/>
+      <c r="AX71" s="60"/>
+      <c r="AY71" s="60"/>
+      <c r="AZ71" s="60"/>
+      <c r="BA71" s="60"/>
+      <c r="BB71" s="61"/>
+      <c r="BC71" s="62"/>
+      <c r="BD71" s="60"/>
+      <c r="BE71" s="60"/>
+      <c r="BF71" s="60"/>
+      <c r="BG71" s="60"/>
+      <c r="BH71" s="60"/>
+      <c r="BI71" s="61"/>
+      <c r="BJ71" s="62"/>
+      <c r="BK71" s="60"/>
+      <c r="BL71" s="60"/>
+      <c r="BM71" s="60"/>
+      <c r="BN71" s="60"/>
+      <c r="BO71" s="60"/>
     </row>
     <row r="72" spans="1:67">
+      <c r="E72" s="7"/>
+      <c r="F72" s="1"/>
       <c r="I72" s="3"/>
     </row>
     <row r="73" spans="1:67">
@@ -8785,68 +9028,74 @@
       <c r="I74" s="3"/>
     </row>
     <row r="75" spans="1:67">
-      <c r="B75" s="8" t="s">
-        <v>94</v>
-      </c>
+      <c r="I75" s="3"/>
     </row>
-    <row r="76" spans="1:67" ht="16.5">
-      <c r="B76" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E76" s="2"/>
-      <c r="F76" s="3"/>
+    <row r="76" spans="1:67">
+      <c r="I76" s="3"/>
     </row>
     <row r="77" spans="1:67">
-      <c r="B77" s="10" t="s">
-        <v>96</v>
+      <c r="B77" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:67">
-      <c r="C78" s="3"/>
+    <row r="78" spans="1:67" ht="16.5">
+      <c r="B78" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" s="3"/>
     </row>
     <row r="79" spans="1:67">
-      <c r="C79" s="3"/>
+      <c r="B79" s="10" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="80" spans="1:67"/>
-    <row r="81" spans="2:8"/>
-    <row r="82" spans="2:8" ht="16.5">
-      <c r="B82" s="2"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+    <row r="80" spans="1:67">
+      <c r="C80" s="3"/>
     </row>
-    <row r="83" spans="2:8">
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+    <row r="81" spans="2:8">
+      <c r="C81" s="3"/>
     </row>
+    <row r="82" spans="2:8"/>
+    <row r="83" spans="2:8"/>
     <row r="84" spans="2:8" ht="16.5">
       <c r="B84" s="2"/>
+      <c r="C84" s="3"/>
       <c r="D84" s="3"/>
     </row>
     <row r="85" spans="2:8">
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
     </row>
-    <row r="86" spans="2:8">
-      <c r="C86" s="3"/>
+    <row r="86" spans="2:8" ht="16.5">
+      <c r="B86" s="2"/>
       <c r="D86" s="3"/>
     </row>
     <row r="87" spans="2:8">
+      <c r="C87" s="3"/>
       <c r="D87" s="3"/>
     </row>
     <row r="88" spans="2:8">
+      <c r="C88" s="3"/>
       <c r="D88" s="3"/>
-      <c r="H88" s="11"/>
     </row>
-    <row r="89" spans="2:8" ht="15" customHeight="1">
+    <row r="89" spans="2:8">
       <c r="D89" s="3"/>
     </row>
-    <row r="90" spans="2:8" ht="15" customHeight="1">
-      <c r="C90" s="3"/>
+    <row r="90" spans="2:8">
       <c r="D90" s="3"/>
+      <c r="H90" s="11"/>
+    </row>
+    <row r="91" spans="2:8" ht="15" customHeight="1">
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="2:8" ht="15" customHeight="1">
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A62:A69"/>
+    <mergeCell ref="A64:A71"/>
     <mergeCell ref="H49:BO49"/>
     <mergeCell ref="H41:BO41"/>
     <mergeCell ref="C1:E1"/>
@@ -8857,7 +9106,7 @@
     <mergeCell ref="B41:G41"/>
     <mergeCell ref="B49:G49"/>
     <mergeCell ref="B17:G17"/>
-    <mergeCell ref="A12:A61"/>
+    <mergeCell ref="A12:A63"/>
     <mergeCell ref="H17:BO17"/>
     <mergeCell ref="H21:BO21"/>
     <mergeCell ref="B53:G53"/>

</xml_diff>